<commit_message>
cleaned up file structure, recreated pathways as necessary
</commit_message>
<xml_diff>
--- a/Data/pokemon_evolution.xlsx
+++ b/Data/pokemon_evolution.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayinsmac/ERHS535_R programming/pokedex/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayinsmac/ERHS535_R programming/pokedex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAE250B-55E7-B441-B370-3B7F84DA4BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC067062-E51E-6B41-928A-4951208444D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{8CA1FD60-6DFD-7A47-BDCB-EE0A23421950}"/>
   </bookViews>
@@ -3116,10 +3116,10 @@
     <t>evolution_two</t>
   </si>
   <si>
-    <t>Nidoran_M</t>
-  </si>
-  <si>
-    <t>Nidoran_F</t>
+    <t>Nidoran_f</t>
+  </si>
+  <si>
+    <t>Nidoran_m</t>
   </si>
 </sst>
 </file>
@@ -3494,8 +3494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA1E258-2644-2941-A326-76C5A4990664}">
   <dimension ref="A1:C569"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3630,7 +3630,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>29</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>31</v>

</xml_diff>